<commit_message>
agent login logout report changes..
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/AgentLoginLogoutReportData.xlsx
+++ b/ocms/src/test/resources/TestData/AgentLoginLogoutReportData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C434AC2-3E14-481A-A541-1855BDA3D4F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2086A7F9-B02C-4310-A31B-A2EC312A10A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="68">
   <si>
     <t>Report Channel</t>
   </si>
@@ -98,6 +98,9 @@
     <t>Delete</t>
   </si>
   <si>
+    <t>y</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -113,6 +116,9 @@
     <t>Is not equal to</t>
   </si>
   <si>
+    <t>QA</t>
+  </si>
+  <si>
     <t>Does not contain</t>
   </si>
   <si>
@@ -122,6 +128,9 @@
     <t>Ends with</t>
   </si>
   <si>
+    <t>Palak Garg</t>
+  </si>
+  <si>
     <t>Team Name</t>
   </si>
   <si>
@@ -179,7 +188,13 @@
     <t xml:space="preserve">Ends with </t>
   </si>
   <si>
+    <t>n</t>
+  </si>
+  <si>
     <t>Agent ID</t>
+  </si>
+  <si>
+    <t>MS</t>
   </si>
   <si>
     <t>SELECT M.[AgentID] as [Agent ID],A.[AgentName] as [Agent Name],[StationID] as [Station ID],
@@ -207,56 +222,44 @@
   order by M.LogoutDateTime ASC;</t>
   </si>
   <si>
+    <t>21-01-2021 00:00:00</t>
+  </si>
+  <si>
+    <t>20-01-2021 00:00:00</t>
+  </si>
+  <si>
+    <t>06-01-2021 00:00:00</t>
+  </si>
+  <si>
+    <t>602</t>
+  </si>
+  <si>
+    <t>Murali</t>
+  </si>
+  <si>
     <t>Supervisor Name</t>
   </si>
   <si>
+    <t>Garg</t>
+  </si>
+  <si>
+    <t>ProductQA</t>
+  </si>
+  <si>
     <t>16-03-2021 00:00:00</t>
   </si>
   <si>
-    <t>Anitha Acharya</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>50011</t>
-  </si>
-  <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
-    <t>Banking</t>
-  </si>
-  <si>
-    <t>Kavitha</t>
-  </si>
-  <si>
-    <t>Hitesh</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Contact Centre</t>
-  </si>
-  <si>
-    <t>01-01-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>18-03-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>30-04-2021 00:00:00</t>
-  </si>
-  <si>
-    <t>03-05-2021 00:00:00</t>
+    <t>01-04-2021 00:00:00</t>
+  </si>
+  <si>
+    <t>08-04-2021 00:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,12 +277,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -605,13 +602,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.81640625" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.7265625" customWidth="1"/>
     <col min="5" max="5" width="16.453125" customWidth="1"/>
@@ -645,7 +642,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -661,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
@@ -704,10 +701,10 @@
         <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>21</v>
@@ -724,10 +721,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -736,7 +733,7 @@
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
         <v>22</v>
@@ -753,10 +750,10 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -765,7 +762,7 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -779,10 +776,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -805,10 +802,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -817,7 +814,7 @@
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -831,19 +828,19 @@
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -857,19 +854,19 @@
         <v>5</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -883,10 +880,10 @@
         <v>5</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -900,10 +897,10 @@
         <v>5</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -917,10 +914,10 @@
         <v>5</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J10" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -934,10 +931,10 @@
         <v>5</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -951,10 +948,10 @@
         <v>5</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -968,10 +965,10 @@
         <v>5</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -985,10 +982,10 @@
         <v>5</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -1002,10 +999,10 @@
         <v>5</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -1019,14 +1016,13 @@
         <v>5</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1036,7 +1032,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1072,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1125,10 +1121,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1141,7 +1137,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1181,7 +1177,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -1197,7 +1193,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1240,10 +1236,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
@@ -1258,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1306,10 +1302,10 @@
         <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1323,10 +1319,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -1338,13 +1334,13 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -1358,25 +1354,25 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1390,22 +1386,22 @@
         <v>5</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
         <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -1419,10 +1415,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
@@ -1431,10 +1427,10 @@
         <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1448,22 +1444,22 @@
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1477,10 +1473,10 @@
         <v>5</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -1489,14 +1485,13 @@
         <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1550,13 +1545,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>